<commit_message>
fixed missing .GBS in gerber package, added zipped releases to gitignore
</commit_message>
<xml_diff>
--- a/Release/Rev-01/Assembly/BOM/Bill of Materials-pai.xlsx
+++ b/Release/Rev-01/Assembly/BOM/Bill of Materials-pai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{143F30DF-2F63-4E76-9622-AE80B5B8EA34}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{454E0722-F9DD-40FC-9007-47296B2CA7B4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="10350" xr2:uid="{CF7A2F26-0CCF-499B-8477-B64145E6E672}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="10350" xr2:uid="{8387FA53-AC6F-4EC1-BBB9-80D8B28E114F}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-pai" sheetId="1" r:id="rId1"/>
@@ -1021,7 +1021,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7FB900-1375-48E8-A8A0-C8F266371EC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4040EBC-5870-4BE3-AEB9-663529E08CF5}">
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2169,44 +2169,44 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" tooltip="Supplier" display="'" xr:uid="{33B591C7-104C-4FE9-BF40-0B10CF855287}"/>
-    <hyperlink ref="H3" tooltip="Supplier" display="'" xr:uid="{8C5761D7-406E-43F8-AA8C-163E313749F1}"/>
-    <hyperlink ref="H4" tooltip="Supplier" display="'" xr:uid="{4084C5BE-9569-4D35-8857-D4F00BA71705}"/>
-    <hyperlink ref="H5" tooltip="Supplier" display="'" xr:uid="{5D0F502B-1E1C-4192-9800-F43562531E0C}"/>
-    <hyperlink ref="H6" tooltip="Supplier" display="'" xr:uid="{D5097D70-AC89-4911-8426-C91FAC867DD1}"/>
-    <hyperlink ref="H7" tooltip="Supplier" display="'" xr:uid="{98395F02-C7AF-4336-99A3-6D6D1CB538F0}"/>
-    <hyperlink ref="H8" tooltip="Supplier" display="'" xr:uid="{DBB6134F-2ADE-4636-B3A1-FECDEC325F74}"/>
-    <hyperlink ref="H9" tooltip="Supplier" display="'" xr:uid="{F29C2DDA-D38E-4205-B01A-123678EA6439}"/>
-    <hyperlink ref="H10" tooltip="Supplier" display="'" xr:uid="{03D98975-8B9A-42B7-8FDE-CD10A51F5CAC}"/>
-    <hyperlink ref="H11" tooltip="Supplier" display="'" xr:uid="{A4B76AB3-97C0-4373-9D92-64B3E0C3D92C}"/>
-    <hyperlink ref="H12" tooltip="Supplier" display="'" xr:uid="{EB2B6EA8-F5F7-4C3E-8320-DFEB885D9A67}"/>
-    <hyperlink ref="H13" tooltip="Supplier" display="'" xr:uid="{2A382492-293E-4E87-934C-FC6A1D7E3E7F}"/>
-    <hyperlink ref="H14" tooltip="Supplier" display="'" xr:uid="{A68CEA0B-2819-4ECA-B620-58BB0A5AAB43}"/>
-    <hyperlink ref="H15" tooltip="Supplier" display="'" xr:uid="{DC293C9C-AB60-4F39-B15F-53F5FFF12AEC}"/>
-    <hyperlink ref="H16" tooltip="Supplier" display="'" xr:uid="{1271B1C7-11D4-4B48-A69D-5A3EDCF2E347}"/>
-    <hyperlink ref="H17" tooltip="Supplier" display="'" xr:uid="{C27203E6-5572-45AC-8924-A2BD1305F761}"/>
-    <hyperlink ref="H18" tooltip="Supplier" display="'" xr:uid="{7D3E2359-AD17-4D4C-840D-EEF8B617FE6E}"/>
-    <hyperlink ref="H19" tooltip="Supplier" display="'" xr:uid="{B792D8FC-FB16-4C4D-906E-DF6C19F378FF}"/>
-    <hyperlink ref="H20" tooltip="Supplier" display="'" xr:uid="{2676D1FC-DA0C-4660-AC5A-07A1459017D4}"/>
-    <hyperlink ref="H21" tooltip="Supplier" display="'" xr:uid="{697D7A21-D602-4143-A823-A6CCF22CDB43}"/>
-    <hyperlink ref="H22" tooltip="Supplier" display="'" xr:uid="{EBE98892-DC0F-4E22-937F-4BE52D3B778D}"/>
-    <hyperlink ref="H23" tooltip="Supplier" display="'" xr:uid="{9D176B30-1471-4291-A28D-177E4A9CFEE1}"/>
-    <hyperlink ref="H24" tooltip="Supplier" display="'" xr:uid="{4DFCEA42-26C6-4CDB-9816-B45E6C1C898B}"/>
-    <hyperlink ref="H25" tooltip="Supplier" display="'" xr:uid="{E47246C3-FAC7-4085-88E1-D30F7CADC725}"/>
-    <hyperlink ref="H26" tooltip="Supplier" display="'" xr:uid="{597CE419-535C-4697-A300-326D19DB41E0}"/>
-    <hyperlink ref="H27" tooltip="Supplier" display="'" xr:uid="{2400018F-06E3-49D2-BA2C-4B0000CC1D0E}"/>
-    <hyperlink ref="H28" tooltip="Supplier" display="'" xr:uid="{40F2E22D-0347-42CB-BCC6-F0B79FD10AE8}"/>
-    <hyperlink ref="H29" tooltip="Supplier" display="'" xr:uid="{DEE12D00-259B-4F01-8589-D138107C3D7D}"/>
-    <hyperlink ref="H30" tooltip="Supplier" display="'" xr:uid="{6E1D0E78-057B-47DF-8E62-8B737BF9AFEB}"/>
-    <hyperlink ref="H31" tooltip="Supplier" display="'" xr:uid="{E2BE8BC9-EDCF-42E7-8CF2-8308A17FAC2B}"/>
-    <hyperlink ref="H32" tooltip="Supplier" display="'" xr:uid="{74D39F4F-D4A5-4DF8-81F6-97DDB3489516}"/>
-    <hyperlink ref="H33" tooltip="Supplier" display="'" xr:uid="{8A67657E-3618-4B5B-82EB-876D0A3867B4}"/>
-    <hyperlink ref="H34" tooltip="Supplier" display="'" xr:uid="{AF2064BD-9EDE-43E2-991A-85EC82DFB036}"/>
-    <hyperlink ref="H35" tooltip="Supplier" display="'" xr:uid="{9CDE2E15-493C-40F4-89F1-6EFD2C22D20E}"/>
-    <hyperlink ref="H36" tooltip="Supplier" display="'" xr:uid="{AC8F9D11-7D2B-43CE-82D7-8CB784CC0F69}"/>
-    <hyperlink ref="H37" tooltip="Supplier" display="'296-1414-5-ND" xr:uid="{6FFC3713-782B-4D73-A544-10BEA82A85C6}"/>
-    <hyperlink ref="H38" tooltip="Supplier" display="'" xr:uid="{DD3C8968-32DA-4805-A4FD-A09EFF9D221E}"/>
-    <hyperlink ref="H39" tooltip="Supplier" display="'296-11107-5-ND" xr:uid="{30877C12-07B3-4BA6-B2E4-F7C19EAC316F}"/>
+    <hyperlink ref="H2" tooltip="Supplier" display="'" xr:uid="{90B93070-C461-4106-AFF3-C6993677CCD1}"/>
+    <hyperlink ref="H3" tooltip="Supplier" display="'" xr:uid="{A3470F5E-CD99-435A-B7B8-E0477F69B9AF}"/>
+    <hyperlink ref="H4" tooltip="Supplier" display="'" xr:uid="{845301B6-760B-4957-AF6E-2B14E0F81759}"/>
+    <hyperlink ref="H5" tooltip="Supplier" display="'" xr:uid="{9EB62609-2DE9-4D74-A285-661F8EE6B3EC}"/>
+    <hyperlink ref="H6" tooltip="Supplier" display="'" xr:uid="{CF31A913-8413-47D8-B37A-4B988D065F9E}"/>
+    <hyperlink ref="H7" tooltip="Supplier" display="'" xr:uid="{D3D7959B-C771-465F-8A9E-B61430EB2C19}"/>
+    <hyperlink ref="H8" tooltip="Supplier" display="'" xr:uid="{A5D600C5-9B85-4CF2-A04F-D71A0222BC44}"/>
+    <hyperlink ref="H9" tooltip="Supplier" display="'" xr:uid="{D0854938-CE22-4DF1-87C0-A19317BE406B}"/>
+    <hyperlink ref="H10" tooltip="Supplier" display="'" xr:uid="{38507455-5E72-40D5-BFFB-CD05F88BCED3}"/>
+    <hyperlink ref="H11" tooltip="Supplier" display="'" xr:uid="{C643DF94-30FD-4D0E-ADF2-CEF2F8028711}"/>
+    <hyperlink ref="H12" tooltip="Supplier" display="'" xr:uid="{151001C3-F0B6-4539-A6A3-DD6A03FB1C24}"/>
+    <hyperlink ref="H13" tooltip="Supplier" display="'" xr:uid="{4E40775F-2CFA-48C8-ABE4-3733155FC7B7}"/>
+    <hyperlink ref="H14" tooltip="Supplier" display="'" xr:uid="{F18542B2-776B-4D63-BD9C-163BBA3CB4F4}"/>
+    <hyperlink ref="H15" tooltip="Supplier" display="'" xr:uid="{B919B48E-843E-49C6-89A8-DDE584DAB247}"/>
+    <hyperlink ref="H16" tooltip="Supplier" display="'" xr:uid="{51F040E6-84DF-41E7-940C-52227F732351}"/>
+    <hyperlink ref="H17" tooltip="Supplier" display="'" xr:uid="{10F1A7AF-9104-4FC3-9C84-DC30C8E215BB}"/>
+    <hyperlink ref="H18" tooltip="Supplier" display="'" xr:uid="{BC8D6A37-C045-4159-81B2-A846A159EA26}"/>
+    <hyperlink ref="H19" tooltip="Supplier" display="'" xr:uid="{24781E8C-58A7-4D70-950C-A5A4549995A9}"/>
+    <hyperlink ref="H20" tooltip="Supplier" display="'" xr:uid="{82959CCD-A0F5-4836-800C-1CA5FEE2D106}"/>
+    <hyperlink ref="H21" tooltip="Supplier" display="'" xr:uid="{78A19DAD-2578-469C-9800-5A14B0BAD8EA}"/>
+    <hyperlink ref="H22" tooltip="Supplier" display="'" xr:uid="{82F58BA0-5507-4B13-A880-03A6ED82CF06}"/>
+    <hyperlink ref="H23" tooltip="Supplier" display="'" xr:uid="{D3D49FFD-42DB-47A4-BEA9-7805051A3952}"/>
+    <hyperlink ref="H24" tooltip="Supplier" display="'" xr:uid="{30343C0E-DF66-48B8-B124-221DACD38694}"/>
+    <hyperlink ref="H25" tooltip="Supplier" display="'" xr:uid="{78325B18-B0EE-4026-8FC4-AED4130155FF}"/>
+    <hyperlink ref="H26" tooltip="Supplier" display="'" xr:uid="{17D53726-6CEE-41D8-914F-F654F9047AF6}"/>
+    <hyperlink ref="H27" tooltip="Supplier" display="'" xr:uid="{13E3766B-2B62-49BC-BAF7-13A84DB89297}"/>
+    <hyperlink ref="H28" tooltip="Supplier" display="'" xr:uid="{0FEF0DB7-02A8-4A5B-9FD9-176B9F4FFA95}"/>
+    <hyperlink ref="H29" tooltip="Supplier" display="'" xr:uid="{A565E7F2-704F-4B54-8BB1-1DA11EA755F9}"/>
+    <hyperlink ref="H30" tooltip="Supplier" display="'" xr:uid="{36BAACF4-66FA-4EA1-88DC-D45E25329EFC}"/>
+    <hyperlink ref="H31" tooltip="Supplier" display="'" xr:uid="{6EDBF174-4777-4D42-A364-49A3B674832C}"/>
+    <hyperlink ref="H32" tooltip="Supplier" display="'" xr:uid="{2DC4F684-78B8-4224-9906-A7FFA4AE104A}"/>
+    <hyperlink ref="H33" tooltip="Supplier" display="'" xr:uid="{E4E79861-D162-4A4D-929C-FEA8249BC8D2}"/>
+    <hyperlink ref="H34" tooltip="Supplier" display="'" xr:uid="{BD24A946-3B4F-4A9A-9098-447D8074473E}"/>
+    <hyperlink ref="H35" tooltip="Supplier" display="'" xr:uid="{84FF76DA-6438-4C0B-BBFA-F186AE2CF813}"/>
+    <hyperlink ref="H36" tooltip="Supplier" display="'" xr:uid="{CA97BF49-E27B-4C3A-AF1C-BC0296349744}"/>
+    <hyperlink ref="H37" tooltip="Supplier" display="'296-1414-5-ND" xr:uid="{77D3CAB2-AA2C-406B-919E-E37861F2F12C}"/>
+    <hyperlink ref="H38" tooltip="Supplier" display="'" xr:uid="{E27C992F-85E7-4C95-AF2E-56134AFB45B6}"/>
+    <hyperlink ref="H39" tooltip="Supplier" display="'296-11107-5-ND" xr:uid="{8B66E60D-C640-4E26-8C6A-F9746AC75D0C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>